<commit_message>
woohoo presentation changes i think
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bengoldman/science-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC548C4-FEC9-B742-BA0F-5ED2DA2BC6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B445BE57-5B02-3B40-BD41-3148BF26CB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{EBC8E4BC-03EE-E74B-A2A7-FD254B5A916A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>presentation lesson</t>
+  </si>
+  <si>
+    <t>worked on jshs form</t>
+  </si>
+  <si>
+    <t>presented</t>
   </si>
 </sst>
 </file>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E183CDD-614A-4043-B604-DC6D735E5831}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,6 +1272,60 @@
         <v>31</v>
       </c>
     </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>44497</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" ref="D44" si="9">C44-B44</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>44498</v>
+      </c>
+      <c r="B45" s="2">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="D45" s="2">
+        <f t="shared" ref="D45" si="10">C45-B45</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B46" s="2">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="D46" s="2">
+        <f t="shared" ref="D46" si="11">C46-B46</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed some figs, edited presentation
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bengoldman/science-research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B445BE57-5B02-3B40-BD41-3148BF26CB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CBD3FC-4E92-2145-AA60-22D255D4808E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{EBC8E4BC-03EE-E74B-A2A7-FD254B5A916A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -136,16 +136,38 @@
   </si>
   <si>
     <t>presented</t>
+  </si>
+  <si>
+    <t>marcus's presentation</t>
+  </si>
+  <si>
+    <t>Jimena's presentation</t>
+  </si>
+  <si>
+    <t>Sarah's presentation</t>
+  </si>
+  <si>
+    <t>Emailed mentor</t>
+  </si>
+  <si>
+    <t>worked on STS application, helped sean with STS application</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,11 +193,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E183CDD-614A-4043-B604-DC6D735E5831}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,8 +538,8 @@
         <v>4</v>
       </c>
       <c r="J1" s="2">
-        <f>SUM(D24:D40)</f>
-        <v>0.70624999999999982</v>
+        <f>SUM(D41:D55)</f>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1319,11 +1342,119 @@
         <v>0.4145833333333333</v>
       </c>
       <c r="D46" s="2">
-        <f t="shared" ref="D46" si="11">C46-B46</f>
+        <f t="shared" ref="D46:D52" si="11">C46-B46</f>
         <v>3.125E-2</v>
       </c>
       <c r="E46" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="11"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>44503</v>
+      </c>
+      <c r="B48" s="4">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" si="11"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>44503</v>
+      </c>
+      <c r="B49" s="4">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" si="11"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>44504</v>
+      </c>
+      <c r="B50" s="4">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" si="11"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B51" s="4">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" si="11"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>44507</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" si="11"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>